<commit_message>
update example with new speciation code
</commit_message>
<xml_diff>
--- a/examples/OregonNd/model_parsing_diagnostics.OregonNd.xlsx
+++ b/examples/OregonNd/model_parsing_diagnostics.OregonNd.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="545">
   <si>
     <t>label</t>
   </si>
@@ -47,7 +47,7 @@
     <t>role</t>
   </si>
   <si>
-    <t>species_modelled</t>
+    <t>formula</t>
   </si>
   <si>
     <t>codename</t>
@@ -134,7 +134,7 @@
     <t>rNC</t>
   </si>
   <si>
-    <t>TNH4,NH4_ads,NH4</t>
+    <t>TNH4,NH4{+},NH4_ads,TNH4_ads,TNH4_ads_nsf,TNH4_dis</t>
   </si>
   <si>
     <t>TNH4</t>
@@ -194,7 +194,7 @@
     <t>+2</t>
   </si>
   <si>
-    <t>TMn,Mn{2+}/Mn_free,Mn_ads_Mn,Mn_ads_Fe</t>
+    <t>TMn,Mn{2+}/Mn_aq,Mn(OH){+}/Mn_OH_aq,Mn(OH)[2]/Mn_OH_2_aq,MnHCO3{+}/MnHCO3_aq,MnCO3/MnCO3_aq,MnSO4/MnSO4_aq,MnCl{+}/MnCl_aq,TMn_dis,Mn_ads_Mn,Mn_ads_Fe,TMn_ads,TMn_ads_MnO2,TMn_ads_FeOOH</t>
   </si>
   <si>
     <t>TMn</t>
@@ -218,7 +218,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>TFe,Fe{2+}/Fe_free,Fe_ads_Mn,Fe_ads_Fe</t>
+    <t>TFe,Fe{2+}/Fe_aq,Fe(OH){+}/Fe_OH_aq,Fe(OH)[2]/Fe_OH_2_aq,FeHCO3{+}/FeHCO3_aq,(FeCO3)/FeCO3_aq,Fe(CO3)[2]{2-}/Fe_CO3_2_aq,FeSO4/FeSO4_aq,FeCl{+}/FeCl_aq,(FeS)[1]/FeS_aq,TFe_dis,Fe_ads_Mn,Fe_ads_Fe,TFe_ads,TFe_ads_MnO2,TFe_ads_FeOOH</t>
   </si>
   <si>
     <t>TFe</t>
@@ -359,7 +359,7 @@
     <t>rAlSi</t>
   </si>
   <si>
-    <t>Al,Al{3+}/Al_free</t>
+    <t>Al,Al{3+}/Al_aq,Al(OH){2+}/Al_OH_aq,Al(OH)[2]{+}/Al_OH_2_aq,Al(OH)[3]/Al_OH_3_aq,Al(OH)[4]{-}/Al_OH_4_aq,Al_dis</t>
   </si>
   <si>
     <t>RMnRe_Ndnr</t>
@@ -371,7 +371,7 @@
     <t>Ndnr</t>
   </si>
   <si>
-    <t>TNdnr,Ndnr{3+}/Ndnr_free,Ndnr,Ndnr_ads_Mn,Ndnr_ads_Fe</t>
+    <t>TNdnr,Ndnr{3+}/Ndnr_aq,NdnrCO3{+}/NdnrCO3_aq,Ndnr(CO3)[2]{-}/Ndnr_CO3_2_aq,NdnrHCO3{2+}/NdnrHCO3_aq,NdnrCl{2+}/NdnrCl_aq,NdnrSO4{+}/NdnrSO4_aq,NdnrOH{2+}/NdnrOH_aq,NdnrH3SiO4{2+}/NdnrH3SiO4_aq,Ndnr(H3SiO4)[2]{+}/Ndnr_H3SiO4_2_aq,TNdnr_dis,Ndnr_ads_Mn,Ndnr_ads_Fe,TNdnr_ads,TNdnr_ads_MnO2,TNdnr_ads_FeOOH</t>
   </si>
   <si>
     <t>TNdnr</t>
@@ -386,7 +386,7 @@
     <t>Ndr</t>
   </si>
   <si>
-    <t>TNdr,Ndr{3+}/Ndr_free,Ndr,Ndr_ads_Mn,Ndr_ads_Fe</t>
+    <t>TNdr,Ndr{3+}/Ndr_aq,NdrCO3{+}/NdrCO3_aq,Ndr(CO3)[2]{-}/Ndr_CO3_2_aq,NdrHCO3{2+}/NdrHCO3_aq,NdrCl{2+}/NdrCl_aq,NdrSO4{+}/NdrSO4_aq,NdrOH{2+}/NdrOH_aq,NdrH3SiO4{2+}/NdrH3SiO4_aq,Ndr(H3SiO4)[2]{+}/Ndr_H3SiO4_2_aq,TNdr_dis,Ndr_ads_Mn,Ndr_ads_Fe,TNdr_ads,TNdr_ads_MnO2,TNdr_ads_FeOOH</t>
   </si>
   <si>
     <t>TNdr</t>
@@ -629,7 +629,7 @@
     <t>dependence</t>
   </si>
   <si>
-    <t>H,TCO2,TH2S,TH4SiO4,TH3PO4,TFe,FeOOH,MnO2,TNdnr,TNdr,TNH4,TMn,SO4,Al,Ca,O2,Age,POC,NO2,NO3,FeS,CH4,CaCO3,NdnrPO4,NdrPO4,Illite,Basalt</t>
+    <t>H,TCO2,TH2S,TH4SiO4,TH3PO4,TMn,FeOOH,MnO2,TFe,Al,TNdnr,TNdr,SO4,TNH4,Ca,NdnrPO4,NdrPO4,O2,Age,POC,NO2,NO3,FeS,CH4,CaCO3,Illite,Basalt</t>
   </si>
   <si>
     <t>H,TCO2,TH2S,TFe,FeOOH,MnO2,SO4,O2,FeS</t>
@@ -641,10 +641,10 @@
     <t>H,TCO2,TH2S,TFe,FeOOH,MnO2,SO4,NO3,NO2,O2,Age,POC,CH4,FeS</t>
   </si>
   <si>
-    <t>H,TCO2,TH4SiO4,TH3PO4,TNdnr,FeOOH,MnO2,TMn,TFe,Al,SO4,NO3,NO2,O2,Age,POC,TH2S,Basalt,SurfMn_Ndnr,SurfFe_Ndnr,NdnrPO4,NdrPO4</t>
-  </si>
-  <si>
-    <t>H,TCO2,TH4SiO4,TH3PO4,TNdr,FeOOH,MnO2,TMn,TFe,Al,SO4,NO3,NO2,O2,Age,POC,TH2S,Basalt,SurfMn_Ndr,SurfFe_Ndr,NdrPO4,NdnrPO4</t>
+    <t>H,TCO2,TH4SiO4,TH3PO4,TMn,FeOOH,MnO2,TFe,Al,TNdnr,SO4,NdnrPO4,NdrPO4,NO3,NO2,O2,Age,POC,TH2S,Basalt,SurfMn_Ndnr,SurfFe_Ndnr</t>
+  </si>
+  <si>
+    <t>H,TCO2,TH4SiO4,TH3PO4,TMn,FeOOH,MnO2,TFe,Al,TNdr,SO4,NdrPO4,NdnrPO4,NO3,NO2,O2,Age,POC,TH2S,Basalt,SurfMn_Ndr,SurfFe_Ndr</t>
   </si>
   <si>
     <t>H,TH4SiO4,Al,Basalt</t>
@@ -656,7 +656,7 @@
     <t>H,TH4SiO4,Al,Illite</t>
   </si>
   <si>
-    <t>H,TCO2,TH4SiO4,TH3PO4,TNdnr,FeOOH,MnO2,TNdr,SO4,O2,Age,POC,NO2,NO3,NdnrPO4,NdrPO4</t>
+    <t>H,TCO2,TH4SiO4,TH3PO4,TNdnr,FeOOH,MnO2,TNdr,SO4,NdnrPO4,NdrPO4,O2,Age,POC,NO2,NO3</t>
   </si>
   <si>
     <t>H,TCO2,TH4SiO4,TH3PO4,TNdnr,FeOOH,MnO2,SO4,NdnrPO4,NdrPO4</t>
@@ -677,13 +677,19 @@
     <t>TMn,FeOOH,MnO2,TFe,TNdr,NO3,NO2,O2,Age,POC,TH2S,SurfMn_Ndr</t>
   </si>
   <si>
+    <t>TMn,FeOOH,MnO2,TFe,TNH4,O2,Age,POC,NO2,TH2S,FeS,CH4</t>
+  </si>
+  <si>
+    <t>TMn,FeOOH,MnO2,TFe,NO3,NO2,O2,Age,POC,TH2S</t>
+  </si>
+  <si>
     <t>TFe,FeOOH,MnO2,TNdnr,NO3,NO2,O2,Age,POC,TH2S,SurfFe_Ndnr</t>
   </si>
   <si>
     <t>TFe,FeOOH,MnO2,TNdr,NO3,NO2,O2,Age,POC,TH2S,SurfFe_Ndr</t>
   </si>
   <si>
-    <t>TNH4,TMn,FeOOH,MnO2,TFe,O2,Age,POC,NO2,TH2S,FeS,CH4</t>
+    <t>TFe,FeOOH,MnO2,NO3,NO2,O2,Age,POC,FeS,TH2S</t>
   </si>
   <si>
     <t>TNH4,O2,Age,POC,NO2,NO3,MnO2,FeOOH,SO4</t>
@@ -692,12 +698,6 @@
     <t>TNH4,NO2,O2,Age,POC,NO3</t>
   </si>
   <si>
-    <t>TMn,FeOOH,MnO2,TFe,NO3,NO2,O2,Age,POC,TH2S</t>
-  </si>
-  <si>
-    <t>TFe,FeOOH,MnO2,NO3,NO2,O2,Age,POC,FeS,TH2S</t>
-  </si>
-  <si>
     <t>TH4SiO4,BSi</t>
   </si>
   <si>
@@ -893,9 +893,6 @@
     <t>AmCa</t>
   </si>
   <si>
-    <t>AmAl</t>
-  </si>
-  <si>
     <t>AmSO4</t>
   </si>
   <si>
@@ -941,46 +938,49 @@
     <t>AmOH</t>
   </si>
   <si>
-    <t>AmMn</t>
-  </si>
-  <si>
-    <t>AmMn_ads_Fe</t>
-  </si>
-  <si>
-    <t>AmMn_ads_Mn</t>
-  </si>
-  <si>
-    <t>AmFe</t>
-  </si>
-  <si>
-    <t>AmFe_ads_Fe</t>
-  </si>
-  <si>
-    <t>AmFe_ads_Mn</t>
-  </si>
-  <si>
-    <t>AmNH4</t>
-  </si>
-  <si>
-    <t>AmNH4_ads</t>
-  </si>
-  <si>
-    <t>AmNdnr</t>
-  </si>
-  <si>
-    <t>AmNdnr_ads_Fe</t>
-  </si>
-  <si>
-    <t>AmNdnr_ads_Mn</t>
-  </si>
-  <si>
-    <t>AmNdr</t>
-  </si>
-  <si>
-    <t>AmNdr_ads_Fe</t>
-  </si>
-  <si>
-    <t>AmNdr_ads_Mn</t>
+    <t>AmTMn_dis</t>
+  </si>
+  <si>
+    <t>AmTMn_ads_MnO2</t>
+  </si>
+  <si>
+    <t>AmTMn_ads_FeOOH</t>
+  </si>
+  <si>
+    <t>AmTFe_dis</t>
+  </si>
+  <si>
+    <t>AmTFe_ads_MnO2</t>
+  </si>
+  <si>
+    <t>AmTFe_ads_FeOOH</t>
+  </si>
+  <si>
+    <t>AmAl_dis</t>
+  </si>
+  <si>
+    <t>AmTNH4_dis</t>
+  </si>
+  <si>
+    <t>AmTNH4_ads_nsf</t>
+  </si>
+  <si>
+    <t>AmTNdnr_dis</t>
+  </si>
+  <si>
+    <t>AmTNdnr_ads_MnO2</t>
+  </si>
+  <si>
+    <t>AmTNdnr_ads_FeOOH</t>
+  </si>
+  <si>
+    <t>AmTNdr_dis</t>
+  </si>
+  <si>
+    <t>AmTNdr_ads_MnO2</t>
+  </si>
+  <si>
+    <t>AmTNdr_ads_FeOOH</t>
   </si>
   <si>
     <t>BcAmMnO2</t>
@@ -1112,12 +1112,6 @@
     <t>BcCmCa</t>
   </si>
   <si>
-    <t>BcAmAl</t>
-  </si>
-  <si>
-    <t>BcCmAl</t>
-  </si>
-  <si>
     <t>BcAmSO4</t>
   </si>
   <si>
@@ -1211,88 +1205,94 @@
     <t>BcCmOH</t>
   </si>
   <si>
-    <t>BcAmMn</t>
-  </si>
-  <si>
-    <t>BcCmMn</t>
-  </si>
-  <si>
-    <t>BcAmMn_ads_Fe</t>
-  </si>
-  <si>
-    <t>BcCmMn_ads_Fe</t>
-  </si>
-  <si>
-    <t>BcAmMn_ads_Mn</t>
-  </si>
-  <si>
-    <t>BcCmMn_ads_Mn</t>
-  </si>
-  <si>
-    <t>BcAmFe</t>
-  </si>
-  <si>
-    <t>BcCmFe</t>
-  </si>
-  <si>
-    <t>BcAmFe_ads_Fe</t>
-  </si>
-  <si>
-    <t>BcCmFe_ads_Fe</t>
-  </si>
-  <si>
-    <t>BcAmFe_ads_Mn</t>
-  </si>
-  <si>
-    <t>BcCmFe_ads_Mn</t>
-  </si>
-  <si>
-    <t>BcAmNH4</t>
-  </si>
-  <si>
-    <t>BcCmNH4</t>
-  </si>
-  <si>
-    <t>BcAmNH4_ads</t>
-  </si>
-  <si>
-    <t>BcCmNH4_ads</t>
-  </si>
-  <si>
-    <t>BcAmNdnr</t>
-  </si>
-  <si>
-    <t>BcCmNdnr</t>
-  </si>
-  <si>
-    <t>BcAmNdnr_ads_Fe</t>
-  </si>
-  <si>
-    <t>BcCmNdnr_ads_Fe</t>
-  </si>
-  <si>
-    <t>BcAmNdnr_ads_Mn</t>
-  </si>
-  <si>
-    <t>BcCmNdnr_ads_Mn</t>
-  </si>
-  <si>
-    <t>BcAmNdr</t>
-  </si>
-  <si>
-    <t>BcCmNdr</t>
-  </si>
-  <si>
-    <t>BcAmNdr_ads_Fe</t>
-  </si>
-  <si>
-    <t>BcCmNdr_ads_Fe</t>
-  </si>
-  <si>
-    <t>BcAmNdr_ads_Mn</t>
-  </si>
-  <si>
-    <t>BcCmNdr_ads_Mn</t>
+    <t>BcAmTMn_dis</t>
+  </si>
+  <si>
+    <t>BcCmTMn_dis</t>
+  </si>
+  <si>
+    <t>BcAmTMn_ads_MnO2</t>
+  </si>
+  <si>
+    <t>BcCmTMn_ads_MnO2</t>
+  </si>
+  <si>
+    <t>BcAmTMn_ads_FeOOH</t>
+  </si>
+  <si>
+    <t>BcCmTMn_ads_FeOOH</t>
+  </si>
+  <si>
+    <t>BcAmTFe_dis</t>
+  </si>
+  <si>
+    <t>BcCmTFe_dis</t>
+  </si>
+  <si>
+    <t>BcAmTFe_ads_MnO2</t>
+  </si>
+  <si>
+    <t>BcCmTFe_ads_MnO2</t>
+  </si>
+  <si>
+    <t>BcAmTFe_ads_FeOOH</t>
+  </si>
+  <si>
+    <t>BcCmTFe_ads_FeOOH</t>
+  </si>
+  <si>
+    <t>BcAmAl_dis</t>
+  </si>
+  <si>
+    <t>BcCmAl_dis</t>
+  </si>
+  <si>
+    <t>BcAmTNH4_dis</t>
+  </si>
+  <si>
+    <t>BcCmTNH4_dis</t>
+  </si>
+  <si>
+    <t>BcAmTNH4_ads_nsf</t>
+  </si>
+  <si>
+    <t>BcCmTNH4_ads_nsf</t>
+  </si>
+  <si>
+    <t>BcAmTNdnr_dis</t>
+  </si>
+  <si>
+    <t>BcCmTNdnr_dis</t>
+  </si>
+  <si>
+    <t>BcAmTNdnr_ads_MnO2</t>
+  </si>
+  <si>
+    <t>BcCmTNdnr_ads_MnO2</t>
+  </si>
+  <si>
+    <t>BcAmTNdnr_ads_FeOOH</t>
+  </si>
+  <si>
+    <t>BcCmTNdnr_ads_FeOOH</t>
+  </si>
+  <si>
+    <t>BcAmTNdr_dis</t>
+  </si>
+  <si>
+    <t>BcCmTNdr_dis</t>
+  </si>
+  <si>
+    <t>BcAmTNdr_ads_MnO2</t>
+  </si>
+  <si>
+    <t>BcCmTNdr_ads_MnO2</t>
+  </si>
+  <si>
+    <t>BcAmTNdr_ads_FeOOH</t>
+  </si>
+  <si>
+    <t>BcCmTNdr_ads_FeOOH</t>
   </si>
   <si>
     <t>alpha</t>
@@ -1316,9 +1316,6 @@
     <t>CaBW</t>
   </si>
   <si>
-    <t>AlBW</t>
-  </si>
-  <si>
     <t>SO4BW</t>
   </si>
   <si>
@@ -1364,109 +1361,112 @@
     <t>OHBW</t>
   </si>
   <si>
-    <t>Mn0</t>
-  </si>
-  <si>
-    <t>Fe0</t>
-  </si>
-  <si>
-    <t>NH40</t>
-  </si>
-  <si>
-    <t>Ndnr0</t>
-  </si>
-  <si>
-    <t>Ndr0</t>
+    <t>TMn_dis0</t>
+  </si>
+  <si>
+    <t>TFe_dis0</t>
+  </si>
+  <si>
+    <t>Al_dis0</t>
+  </si>
+  <si>
+    <t>TNH4_dis0</t>
+  </si>
+  <si>
+    <t>TNdnr_dis0</t>
+  </si>
+  <si>
+    <t>TNdr_dis0</t>
+  </si>
+  <si>
+    <t>dstopw</t>
+  </si>
+  <si>
+    <t>adsorption</t>
+  </si>
+  <si>
+    <t>KCO2</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>KHCO3</t>
+  </si>
+  <si>
+    <t>KH2S</t>
+  </si>
+  <si>
+    <t>KH3BO3</t>
+  </si>
+  <si>
+    <t>KH3PO4</t>
+  </si>
+  <si>
+    <t>KH2PO4</t>
+  </si>
+  <si>
+    <t>KHPO4</t>
+  </si>
+  <si>
+    <t>KH2O</t>
+  </si>
+  <si>
+    <t>KH4SiO4</t>
   </si>
   <si>
     <t>KMn_ads_Fe</t>
   </si>
   <si>
-    <t>adsorption</t>
-  </si>
-  <si>
-    <t>dstopw</t>
+    <t>speciation</t>
+  </si>
+  <si>
+    <t>TMn_dis,Mn_ads_Fe</t>
+  </si>
+  <si>
+    <t>TMn_dis,TFe_dis,TNH4_dis,TNdnr_dis,TNdr_dis</t>
   </si>
   <si>
     <t>KMn_ads_Mn</t>
   </si>
   <si>
+    <t>TMn_dis,Mn_ads_Mn</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>Mn_aq,Mn_OH_aq,Mn_OH_2_aq,MnHCO3_aq,MnCO3_aq,MnSO4_aq,MnCl_aq,Fe_aq,Fe_OH_aq,Fe_OH_2_aq,FeHCO3_aq,FeCO3_aq,Fe_CO3_2_aq,FeSO4_aq,FeCl_aq,FeS_aq,Ndnr_aq,NdnrCO3_aq,Ndnr_CO3_2_aq,NdnrHCO3_aq,NdnrCl_aq,NdnrSO4_aq,NdnrOH_aq,NdnrH3SiO4_aq,Ndnr_H3SiO4_2_aq,Ndr_aq,NdrCO3_aq,Ndr_CO3_2_aq,NdrHCO3_aq,NdrCl_aq,NdrSO4_aq,NdrOH_aq,NdrH3SiO4_aq,Ndr_H3SiO4_2_aq</t>
+  </si>
+  <si>
     <t>KFe_ads_Fe</t>
   </si>
   <si>
+    <t>TFe_dis,Fe_ads_Fe</t>
+  </si>
+  <si>
     <t>KFe_ads_Mn</t>
   </si>
   <si>
+    <t>TFe_dis,Fe_ads_Mn</t>
+  </si>
+  <si>
     <t>KNH4_ads</t>
   </si>
   <si>
+    <t>TNH4_dis,NH4_ads</t>
+  </si>
+  <si>
     <t>KNd_ads_Fe</t>
   </si>
   <si>
+    <t>TNdnr_dis,Ndnr_ads_Fe,TNdr_dis,Ndr_ads_Fe</t>
+  </si>
+  <si>
     <t>KNd_ads_Mn</t>
   </si>
   <si>
-    <t>KCO2</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>KHCO3</t>
-  </si>
-  <si>
-    <t>KH2S</t>
-  </si>
-  <si>
-    <t>KH3BO3</t>
-  </si>
-  <si>
-    <t>KH3PO4</t>
-  </si>
-  <si>
-    <t>KH2PO4</t>
-  </si>
-  <si>
-    <t>KHPO4</t>
-  </si>
-  <si>
-    <t>KH2O</t>
-  </si>
-  <si>
-    <t>KH4SiO4</t>
-  </si>
-  <si>
-    <t>Cl</t>
-  </si>
-  <si>
-    <t>speciation</t>
-  </si>
-  <si>
-    <t>Fe_free,Fe_OH_aq,Fe_OH_2_aq,FeHCO3_aq,FeCO3_aq,Fe_CO3_2_aq,FeSO4_aq,FeCl_aq,FeS_aq,Ndnr_free,NdnrCO3_aq,Ndnr_CO3_2_aq,NdnrHCO3_aq,NdnrCl_aq,NdnrSO4_aq,NdnrOH_aq,NdnrH3SiO4_aq,Ndnr_H3SiO4_2_aq,Ndr_free,NdrCO3_aq,Ndr_CO3_2_aq,NdrHCO3_aq,NdrCl_aq,NdrSO4_aq,NdrOH_aq,NdrH3SiO4_aq,Ndr_H3SiO4_2_aq,Mn_free,Mn_OH_aq,Mn_OH_2_aq,MnHCO3_aq,MnCO3_aq,MnSO4_aq,MnCl_aq</t>
-  </si>
-  <si>
-    <t>Mn,Mn_ads_Fe</t>
-  </si>
-  <si>
-    <t>Mn,Fe,NH4,Ndnr,Ndr</t>
-  </si>
-  <si>
-    <t>Mn,Mn_ads_Mn</t>
-  </si>
-  <si>
-    <t>Fe,Fe_ads_Fe</t>
-  </si>
-  <si>
-    <t>Fe,Fe_ads_Mn</t>
-  </si>
-  <si>
-    <t>NH4,NH4_ads</t>
-  </si>
-  <si>
-    <t>Ndnr,Ndnr_ads_Fe,Ndr,Ndr_ads_Fe</t>
-  </si>
-  <si>
-    <t>Ndnr,Ndnr_ads_Mn,Ndr,Ndr_ads_Mn</t>
+    <t>TNdnr_dis,Ndnr_ads_Mn,TNdr_dis,Ndr_ads_Mn</t>
   </si>
   <si>
     <t>KspFeS</t>
@@ -1490,6 +1490,12 @@
     <t>Omega_RBSi_dis</t>
   </si>
   <si>
+    <t>KspNdPO4</t>
+  </si>
+  <si>
+    <t>Omega_RNdnrPO4_pre,Omega_RNdrPO4_pre</t>
+  </si>
+  <si>
     <t>KspBasalt</t>
   </si>
   <si>
@@ -1647,9 +1653,6 @@
   </si>
   <si>
     <t>RNdnrPO4_pre,RNdrPO4_pre</t>
-  </si>
-  <si>
-    <t>KspNdPO4</t>
   </si>
   <si>
     <t>kIllite</t>
@@ -6293,13 +6296,13 @@
         <v>107</v>
       </c>
       <c r="I119" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="J119">
         <v>24</v>
       </c>
       <c r="K119" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="L119" t="s">
         <v>19</v>
@@ -7121,13 +7124,13 @@
         <v>107</v>
       </c>
       <c r="I142" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="J142">
         <v>24</v>
       </c>
       <c r="K142" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="L142" t="s">
         <v>21</v>
@@ -7373,13 +7376,13 @@
         <v>107</v>
       </c>
       <c r="I149" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="J149">
         <v>24</v>
       </c>
       <c r="K149" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="L149" t="s">
         <v>19</v>
@@ -11599,7 +11602,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>215</v>
@@ -11607,7 +11610,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
         <v>216</v>
@@ -11615,39 +11618,39 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
         <v>220</v>
@@ -11655,7 +11658,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
         <v>221</v>
@@ -11716,7 +11719,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:B233"/>
+  <dimension ref="A1:B226"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -13463,63 +13466,63 @@
         <v>451</v>
       </c>
       <c r="B218" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
+        <v>453</v>
+      </c>
+      <c r="B219" t="s">
         <v>452</v>
-      </c>
-      <c r="B219" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B220" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B221" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B222" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B223" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B224" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B225" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -13527,63 +13530,7 @@
         <v>460</v>
       </c>
       <c r="B226" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2">
-      <c r="A227" t="s">
-        <v>461</v>
-      </c>
-      <c r="B227" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2">
-      <c r="A228" t="s">
-        <v>462</v>
-      </c>
-      <c r="B228" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2">
-      <c r="A229" t="s">
-        <v>463</v>
-      </c>
-      <c r="B229" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2">
-      <c r="A230" t="s">
-        <v>464</v>
-      </c>
-      <c r="B230" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2">
-      <c r="A231" t="s">
-        <v>465</v>
-      </c>
-      <c r="B231" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2">
-      <c r="A232" t="s">
-        <v>466</v>
-      </c>
-      <c r="B232" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2">
-      <c r="A233" t="s">
-        <v>467</v>
-      </c>
-      <c r="B233" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -13612,13 +13559,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B2" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="C2" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -13626,84 +13573,84 @@
         <v>449</v>
       </c>
       <c r="B3" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="C3" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>451</v>
+        <v>465</v>
       </c>
       <c r="B4" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="C4" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>452</v>
+        <v>467</v>
       </c>
       <c r="B5" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="C5" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>453</v>
+        <v>469</v>
       </c>
       <c r="B6" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="C6" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>454</v>
+        <v>471</v>
       </c>
       <c r="B7" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="C7" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>455</v>
+        <v>473</v>
       </c>
       <c r="B8" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="C8" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>456</v>
+        <v>475</v>
       </c>
       <c r="B9" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="C9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>457</v>
+        <v>477</v>
       </c>
       <c r="B10" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="C10" t="s">
         <v>478</v>
@@ -13755,10 +13702,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>451</v>
+        <v>488</v>
       </c>
       <c r="B15" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="C15" t="s">
         <v>489</v>
@@ -13766,32 +13713,32 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>449</v>
       </c>
       <c r="B16" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C16" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C17" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>492</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C18" t="s">
         <v>493</v>
@@ -13799,43 +13746,43 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>494</v>
       </c>
       <c r="B19" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C19" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C20" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B21" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C21" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>497</v>
+        <v>150</v>
       </c>
       <c r="B22" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C22" t="s">
         <v>498</v>
@@ -13846,32 +13793,32 @@
         <v>499</v>
       </c>
       <c r="B23" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C23" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>501</v>
+      </c>
+      <c r="B24" t="s">
+        <v>490</v>
+      </c>
+      <c r="C24" t="s">
         <v>500</v>
-      </c>
-      <c r="B24" t="s">
-        <v>488</v>
-      </c>
-      <c r="C24" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B25" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C25" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -13879,7 +13826,7 @@
         <v>503</v>
       </c>
       <c r="B26" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C26" t="s">
         <v>504</v>
@@ -13890,7 +13837,7 @@
         <v>505</v>
       </c>
       <c r="B27" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C27" t="s">
         <v>506</v>
@@ -13901,7 +13848,7 @@
         <v>507</v>
       </c>
       <c r="B28" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C28" t="s">
         <v>508</v>
@@ -13912,7 +13859,7 @@
         <v>509</v>
       </c>
       <c r="B29" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C29" t="s">
         <v>510</v>
@@ -13923,128 +13870,128 @@
         <v>511</v>
       </c>
       <c r="B30" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>512</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B31" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B32" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B33" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B34" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B35" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B36" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B37" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B38" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C38" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B39" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B40" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B41" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C41" t="s">
         <v>88</v>
@@ -14052,87 +13999,87 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B42" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B43" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B44" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B45" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B46" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B47" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B48" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B49" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C49" t="s">
         <v>97</v>
@@ -14140,10 +14087,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B50" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C50" t="s">
         <v>97</v>
@@ -14151,24 +14098,24 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B51" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B52" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C52" t="s">
-        <v>534</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -14176,7 +14123,7 @@
         <v>535</v>
       </c>
       <c r="B53" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C53" t="s">
         <v>536</v>
@@ -14187,7 +14134,7 @@
         <v>537</v>
       </c>
       <c r="B54" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C54" t="s">
         <v>538</v>
@@ -14198,18 +14145,18 @@
         <v>539</v>
       </c>
       <c r="B55" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C55" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B56" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C56" t="s">
         <v>135</v>
@@ -14217,10 +14164,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B57" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C57" t="s">
         <v>135</v>
@@ -14228,10 +14175,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B58" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C58" t="s">
         <v>142</v>
@@ -14239,10 +14186,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B59" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C59" t="s">
         <v>142</v>

</xml_diff>